<commit_message>
Changes to testscripts and adding prod bat file
</commit_message>
<xml_diff>
--- a/User_credentials.xlsx
+++ b/User_credentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alok's\Documents\WebDriverIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97A2A5A-6EF0-4C89-A6BC-344012EE25E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488CA78B-7434-4B50-B7F6-7CF4F64F2EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="20475" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <t>mmishra</t>
   </si>
   <si>
-    <t>password=2</t>
+    <t>password=1</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>